<commit_message>
Patch 1/22 (File CLeanup)
</commit_message>
<xml_diff>
--- a/PREMIER SCHEDULE TEMPLATE.xlsx
+++ b/PREMIER SCHEDULE TEMPLATE.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="78">
   <si>
     <t>VALORANT PREMIER STAGE E8A1</t>
   </si>
@@ -155,18 +155,18 @@
     <t>Maja</t>
   </si>
   <si>
+    <t>Raze (All), Cypher (Sunset, Bind), Omen (All)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Hobxn</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Raze (All), Cypher (Sunset, Bind), Omen (All)</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Hobxn</t>
-  </si>
-  <si>
     <t>All Agents (All Maps)</t>
   </si>
   <si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
   <si>
     <t>QUALIFIED FOR PLAYOFFS:</t>
@@ -2306,77 +2309,77 @@
         <v>46</v>
       </c>
       <c r="B11" s="45" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="46">
         <f t="shared" si="1"/>
         <v>85.71428571</v>
       </c>
       <c r="D11" s="59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" s="60"/>
       <c r="F11" s="60"/>
       <c r="G11" s="60"/>
       <c r="H11" s="61"/>
       <c r="I11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J11" s="51"/>
       <c r="K11" s="51"/>
       <c r="L11" s="51"/>
       <c r="M11" s="52"/>
       <c r="N11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O11" s="51"/>
       <c r="P11" s="51"/>
       <c r="Q11" s="51"/>
       <c r="R11" s="52"/>
       <c r="S11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T11" s="51"/>
       <c r="U11" s="51"/>
       <c r="V11" s="51"/>
       <c r="W11" s="54"/>
       <c r="X11" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Y11" s="51"/>
       <c r="Z11" s="51"/>
       <c r="AA11" s="51"/>
       <c r="AB11" s="52"/>
       <c r="AC11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AD11" s="51"/>
       <c r="AE11" s="51"/>
       <c r="AF11" s="51"/>
       <c r="AG11" s="52"/>
       <c r="AH11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI11" s="51"/>
       <c r="AJ11" s="51"/>
       <c r="AK11" s="51"/>
       <c r="AL11" s="54"/>
       <c r="AM11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AN11" s="51"/>
       <c r="AO11" s="51"/>
       <c r="AP11" s="51"/>
       <c r="AQ11" s="52"/>
       <c r="AR11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AS11" s="51"/>
       <c r="AT11" s="51"/>
       <c r="AU11" s="51"/>
       <c r="AV11" s="52"/>
       <c r="AW11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX11" s="51"/>
       <c r="AY11" s="51"/>
@@ -2398,63 +2401,63 @@
       <c r="BO11" s="51"/>
       <c r="BP11" s="54"/>
       <c r="BQ11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BR11" s="51"/>
       <c r="BS11" s="51"/>
       <c r="BT11" s="51"/>
       <c r="BU11" s="52"/>
       <c r="BV11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BW11" s="51"/>
       <c r="BX11" s="51"/>
       <c r="BY11" s="51"/>
       <c r="BZ11" s="52"/>
       <c r="CA11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CB11" s="51"/>
       <c r="CC11" s="51"/>
       <c r="CD11" s="51"/>
       <c r="CE11" s="54"/>
       <c r="CF11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CG11" s="51"/>
       <c r="CH11" s="51"/>
       <c r="CI11" s="51"/>
       <c r="CJ11" s="52"/>
       <c r="CK11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CL11" s="51"/>
       <c r="CM11" s="51"/>
       <c r="CN11" s="51"/>
       <c r="CO11" s="52"/>
       <c r="CP11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CQ11" s="51"/>
       <c r="CR11" s="51"/>
       <c r="CS11" s="51"/>
       <c r="CT11" s="54"/>
       <c r="CU11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CV11" s="51"/>
       <c r="CW11" s="51"/>
       <c r="CX11" s="51"/>
       <c r="CY11" s="52"/>
       <c r="CZ11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DA11" s="51"/>
       <c r="DB11" s="51"/>
       <c r="DC11" s="51"/>
       <c r="DD11" s="52"/>
       <c r="DE11" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DF11" s="51"/>
       <c r="DG11" s="51"/>
@@ -2468,10 +2471,10 @@
     </row>
     <row r="12" ht="21.0" customHeight="1">
       <c r="A12" s="58" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="45" t="s">
         <v>50</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>43</v>
       </c>
       <c r="C12" s="46">
         <f t="shared" si="1"/>
@@ -2485,147 +2488,147 @@
       <c r="G12" s="60"/>
       <c r="H12" s="61"/>
       <c r="I12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J12" s="51"/>
       <c r="K12" s="51"/>
       <c r="L12" s="51"/>
       <c r="M12" s="52"/>
       <c r="N12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O12" s="51"/>
       <c r="P12" s="51"/>
       <c r="Q12" s="51"/>
       <c r="R12" s="52"/>
       <c r="S12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T12" s="51"/>
       <c r="U12" s="51"/>
       <c r="V12" s="51"/>
       <c r="W12" s="52"/>
       <c r="X12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Y12" s="51"/>
       <c r="Z12" s="51"/>
       <c r="AA12" s="51"/>
       <c r="AB12" s="52"/>
       <c r="AC12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AD12" s="51"/>
       <c r="AE12" s="51"/>
       <c r="AF12" s="51"/>
       <c r="AG12" s="52"/>
       <c r="AH12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI12" s="51"/>
       <c r="AJ12" s="51"/>
       <c r="AK12" s="51"/>
       <c r="AL12" s="52"/>
       <c r="AM12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AN12" s="51"/>
       <c r="AO12" s="51"/>
       <c r="AP12" s="51"/>
       <c r="AQ12" s="52"/>
       <c r="AR12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AS12" s="51"/>
       <c r="AT12" s="51"/>
       <c r="AU12" s="51"/>
       <c r="AV12" s="52"/>
       <c r="AW12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX12" s="51"/>
       <c r="AY12" s="51"/>
       <c r="AZ12" s="51"/>
       <c r="BA12" s="52"/>
       <c r="BB12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC12" s="51"/>
       <c r="BD12" s="51"/>
       <c r="BE12" s="51"/>
       <c r="BF12" s="52"/>
       <c r="BG12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BH12" s="51"/>
       <c r="BI12" s="51"/>
       <c r="BJ12" s="51"/>
       <c r="BK12" s="52"/>
       <c r="BL12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BM12" s="51"/>
       <c r="BN12" s="51"/>
       <c r="BO12" s="51"/>
       <c r="BP12" s="52"/>
       <c r="BQ12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BR12" s="51"/>
       <c r="BS12" s="51"/>
       <c r="BT12" s="51"/>
       <c r="BU12" s="52"/>
       <c r="BV12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BW12" s="51"/>
       <c r="BX12" s="51"/>
       <c r="BY12" s="51"/>
       <c r="BZ12" s="52"/>
       <c r="CA12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CB12" s="51"/>
       <c r="CC12" s="51"/>
       <c r="CD12" s="51"/>
       <c r="CE12" s="52"/>
       <c r="CF12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CG12" s="51"/>
       <c r="CH12" s="51"/>
       <c r="CI12" s="51"/>
       <c r="CJ12" s="52"/>
       <c r="CK12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CL12" s="51"/>
       <c r="CM12" s="51"/>
       <c r="CN12" s="51"/>
       <c r="CO12" s="52"/>
       <c r="CP12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CQ12" s="51"/>
       <c r="CR12" s="51"/>
       <c r="CS12" s="51"/>
       <c r="CT12" s="52"/>
       <c r="CU12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CV12" s="51"/>
       <c r="CW12" s="51"/>
       <c r="CX12" s="51"/>
       <c r="CY12" s="52"/>
       <c r="CZ12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DA12" s="51"/>
       <c r="DB12" s="51"/>
       <c r="DC12" s="51"/>
       <c r="DD12" s="52"/>
       <c r="DE12" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DF12" s="51"/>
       <c r="DG12" s="51"/>
@@ -2813,7 +2816,7 @@
       <c r="G14" s="60"/>
       <c r="H14" s="61"/>
       <c r="I14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J14" s="51"/>
       <c r="K14" s="51"/>
@@ -2825,14 +2828,14 @@
       <c r="Q14" s="51"/>
       <c r="R14" s="52"/>
       <c r="S14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T14" s="51"/>
       <c r="U14" s="51"/>
       <c r="V14" s="51"/>
       <c r="W14" s="54"/>
       <c r="X14" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Y14" s="51"/>
       <c r="Z14" s="51"/>
@@ -2844,14 +2847,14 @@
       <c r="AF14" s="51"/>
       <c r="AG14" s="52"/>
       <c r="AH14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI14" s="51"/>
       <c r="AJ14" s="51"/>
       <c r="AK14" s="51"/>
       <c r="AL14" s="54"/>
       <c r="AM14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AN14" s="51"/>
       <c r="AO14" s="51"/>
@@ -2863,14 +2866,14 @@
       <c r="AU14" s="51"/>
       <c r="AV14" s="52"/>
       <c r="AW14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX14" s="51"/>
       <c r="AY14" s="51"/>
       <c r="AZ14" s="51"/>
       <c r="BA14" s="54"/>
       <c r="BB14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC14" s="51"/>
       <c r="BD14" s="51"/>
@@ -2897,14 +2900,14 @@
       <c r="BY14" s="51"/>
       <c r="BZ14" s="52"/>
       <c r="CA14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CB14" s="51"/>
       <c r="CC14" s="51"/>
       <c r="CD14" s="51"/>
       <c r="CE14" s="54"/>
       <c r="CF14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CG14" s="51"/>
       <c r="CH14" s="51"/>
@@ -2916,28 +2919,28 @@
       <c r="CN14" s="51"/>
       <c r="CO14" s="52"/>
       <c r="CP14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CQ14" s="51"/>
       <c r="CR14" s="51"/>
       <c r="CS14" s="51"/>
       <c r="CT14" s="54"/>
       <c r="CU14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CV14" s="51"/>
       <c r="CW14" s="51"/>
       <c r="CX14" s="51"/>
       <c r="CY14" s="52"/>
       <c r="CZ14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DA14" s="51"/>
       <c r="DB14" s="51"/>
       <c r="DC14" s="51"/>
       <c r="DD14" s="52"/>
       <c r="DE14" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DF14" s="51"/>
       <c r="DG14" s="51"/>
@@ -2968,63 +2971,63 @@
       <c r="G15" s="60"/>
       <c r="H15" s="61"/>
       <c r="I15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J15" s="51"/>
       <c r="K15" s="51"/>
       <c r="L15" s="51"/>
       <c r="M15" s="52"/>
       <c r="N15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O15" s="51"/>
       <c r="P15" s="51"/>
       <c r="Q15" s="51"/>
       <c r="R15" s="52"/>
       <c r="S15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T15" s="51"/>
       <c r="U15" s="51"/>
       <c r="V15" s="51"/>
       <c r="W15" s="54"/>
       <c r="X15" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Y15" s="51"/>
       <c r="Z15" s="51"/>
       <c r="AA15" s="51"/>
       <c r="AB15" s="52"/>
       <c r="AC15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AD15" s="51"/>
       <c r="AE15" s="51"/>
       <c r="AF15" s="51"/>
       <c r="AG15" s="52"/>
       <c r="AH15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI15" s="51"/>
       <c r="AJ15" s="51"/>
       <c r="AK15" s="51"/>
       <c r="AL15" s="54"/>
       <c r="AM15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AN15" s="51"/>
       <c r="AO15" s="51"/>
       <c r="AP15" s="51"/>
       <c r="AQ15" s="52"/>
       <c r="AR15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AS15" s="51"/>
       <c r="AT15" s="51"/>
       <c r="AU15" s="51"/>
       <c r="AV15" s="52"/>
       <c r="AW15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX15" s="51"/>
       <c r="AY15" s="51"/>
@@ -3046,63 +3049,63 @@
       <c r="BO15" s="51"/>
       <c r="BP15" s="54"/>
       <c r="BQ15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BR15" s="51"/>
       <c r="BS15" s="51"/>
       <c r="BT15" s="51"/>
       <c r="BU15" s="52"/>
       <c r="BV15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BW15" s="51"/>
       <c r="BX15" s="51"/>
       <c r="BY15" s="51"/>
       <c r="BZ15" s="52"/>
       <c r="CA15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CB15" s="51"/>
       <c r="CC15" s="51"/>
       <c r="CD15" s="51"/>
       <c r="CE15" s="54"/>
       <c r="CF15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CG15" s="51"/>
       <c r="CH15" s="51"/>
       <c r="CI15" s="51"/>
       <c r="CJ15" s="52"/>
       <c r="CK15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CL15" s="51"/>
       <c r="CM15" s="51"/>
       <c r="CN15" s="51"/>
       <c r="CO15" s="52"/>
       <c r="CP15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CQ15" s="51"/>
       <c r="CR15" s="51"/>
       <c r="CS15" s="51"/>
       <c r="CT15" s="54"/>
       <c r="CU15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CV15" s="51"/>
       <c r="CW15" s="51"/>
       <c r="CX15" s="51"/>
       <c r="CY15" s="52"/>
       <c r="CZ15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DA15" s="51"/>
       <c r="DB15" s="51"/>
       <c r="DC15" s="51"/>
       <c r="DD15" s="52"/>
       <c r="DE15" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DF15" s="51"/>
       <c r="DG15" s="51"/>
@@ -3146,126 +3149,126 @@
       <c r="V16" s="51"/>
       <c r="W16" s="54"/>
       <c r="X16" s="62" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Y16" s="51"/>
       <c r="Z16" s="51"/>
       <c r="AA16" s="51"/>
       <c r="AB16" s="52"/>
       <c r="AC16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AD16" s="51"/>
       <c r="AE16" s="51"/>
       <c r="AF16" s="51"/>
       <c r="AG16" s="52"/>
       <c r="AH16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AI16" s="51"/>
       <c r="AJ16" s="51"/>
       <c r="AK16" s="51"/>
       <c r="AL16" s="54"/>
       <c r="AM16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AN16" s="51"/>
       <c r="AO16" s="51"/>
       <c r="AP16" s="51"/>
       <c r="AQ16" s="52"/>
       <c r="AR16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AS16" s="51"/>
       <c r="AT16" s="51"/>
       <c r="AU16" s="51"/>
       <c r="AV16" s="52"/>
       <c r="AW16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX16" s="51"/>
       <c r="AY16" s="51"/>
       <c r="AZ16" s="51"/>
       <c r="BA16" s="54"/>
       <c r="BB16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC16" s="51"/>
       <c r="BD16" s="51"/>
       <c r="BE16" s="51"/>
       <c r="BF16" s="52"/>
       <c r="BG16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BH16" s="51"/>
       <c r="BI16" s="51"/>
       <c r="BJ16" s="51"/>
       <c r="BK16" s="52"/>
       <c r="BL16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BM16" s="51"/>
       <c r="BN16" s="51"/>
       <c r="BO16" s="51"/>
       <c r="BP16" s="54"/>
       <c r="BQ16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BR16" s="51"/>
       <c r="BS16" s="51"/>
       <c r="BT16" s="51"/>
       <c r="BU16" s="52"/>
       <c r="BV16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BW16" s="51"/>
       <c r="BX16" s="51"/>
       <c r="BY16" s="51"/>
       <c r="BZ16" s="52"/>
       <c r="CA16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CB16" s="51"/>
       <c r="CC16" s="51"/>
       <c r="CD16" s="51"/>
       <c r="CE16" s="54"/>
       <c r="CF16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CG16" s="51"/>
       <c r="CH16" s="51"/>
       <c r="CI16" s="51"/>
       <c r="CJ16" s="52"/>
       <c r="CK16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CL16" s="51"/>
       <c r="CM16" s="51"/>
       <c r="CN16" s="51"/>
       <c r="CO16" s="52"/>
       <c r="CP16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CQ16" s="51"/>
       <c r="CR16" s="51"/>
       <c r="CS16" s="51"/>
       <c r="CT16" s="54"/>
       <c r="CU16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CV16" s="51"/>
       <c r="CW16" s="51"/>
       <c r="CX16" s="51"/>
       <c r="CY16" s="52"/>
       <c r="CZ16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DA16" s="51"/>
       <c r="DB16" s="51"/>
       <c r="DC16" s="51"/>
       <c r="DD16" s="52"/>
       <c r="DE16" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="DF16" s="51"/>
       <c r="DG16" s="51"/>
@@ -3282,11 +3285,11 @@
         <v>60</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C17" s="46">
         <f t="shared" si="1"/>
-        <v>28.57142857</v>
+        <v>23.80952381</v>
       </c>
       <c r="D17" s="59" t="s">
         <v>61</v>
@@ -3296,21 +3299,19 @@
       <c r="G17" s="60"/>
       <c r="H17" s="61"/>
       <c r="I17" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J17" s="51"/>
       <c r="K17" s="51"/>
       <c r="L17" s="51"/>
       <c r="M17" s="52"/>
-      <c r="N17" s="53" t="s">
-        <v>49</v>
-      </c>
+      <c r="N17" s="53"/>
       <c r="O17" s="51"/>
       <c r="P17" s="51"/>
       <c r="Q17" s="51"/>
       <c r="R17" s="52"/>
       <c r="S17" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T17" s="51"/>
       <c r="U17" s="51"/>
@@ -3332,7 +3333,7 @@
       <c r="AK17" s="51"/>
       <c r="AL17" s="54"/>
       <c r="AM17" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AN17" s="51"/>
       <c r="AO17" s="51"/>
@@ -3349,7 +3350,7 @@
       <c r="AZ17" s="51"/>
       <c r="BA17" s="54"/>
       <c r="BB17" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BC17" s="51"/>
       <c r="BD17" s="51"/>
@@ -3396,7 +3397,7 @@
       <c r="CS17" s="51"/>
       <c r="CT17" s="54"/>
       <c r="CU17" s="53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="CV17" s="51"/>
       <c r="CW17" s="51"/>
@@ -3678,7 +3679,7 @@
       <c r="M20" s="76"/>
       <c r="N20" s="77">
         <f>COUNTIF(N10:R19, "X")</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R20" s="76"/>
       <c r="S20" s="77">
@@ -3988,7 +3989,7 @@
       <c r="M22" s="83"/>
       <c r="N22" s="82" t="b">
         <f>AND(N20 &gt;5)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" s="72"/>
       <c r="P22" s="72"/>
@@ -4185,7 +4186,6 @@
 Hobxn
 Log
 Meeko
-Ink
 </v>
       </c>
       <c r="O23" s="72"/>
@@ -4744,7 +4744,9 @@
         <v>73</v>
       </c>
       <c r="R28" s="76"/>
-      <c r="S28" s="97"/>
+      <c r="S28" s="97" t="s">
+        <v>74</v>
+      </c>
       <c r="W28" s="76"/>
       <c r="X28" s="97"/>
       <c r="AB28" s="76"/>
@@ -4798,7 +4800,6 @@
 Hobxn
 Log
 Meeko
-Ink
 </v>
       </c>
       <c r="D29" s="61"/>
@@ -4809,7 +4810,7 @@
       <c r="F29" s="61"/>
       <c r="G29" s="95" t="str">
         <f>S28</f>
-        <v/>
+        <v>W</v>
       </c>
       <c r="H29" s="61"/>
       <c r="I29" s="65"/>
@@ -4827,7 +4828,7 @@
       <c r="R29" s="83"/>
       <c r="S29" s="82">
         <f>IF(S28="L", 25, IF(S28="", 0, 100))</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="T29" s="72"/>
       <c r="U29" s="72"/>
@@ -5018,7 +5019,7 @@
       <c r="K30" s="65"/>
       <c r="L30" s="65"/>
       <c r="N30" s="98" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O30" s="99"/>
       <c r="P30" s="99"/>
@@ -5086,7 +5087,7 @@
       <c r="K31" s="65"/>
       <c r="L31" s="65"/>
       <c r="N31" s="102" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O31" s="103"/>
       <c r="P31" s="103"/>
@@ -5103,8 +5104,8 @@
       <c r="AA31" s="103"/>
       <c r="AB31" s="104"/>
       <c r="AC31" s="101">
-        <f>IF(650 - SUM(N29:DN29)&lt;0, 0, 650 - SUM(N29:DN29))</f>
-        <v>625</v>
+        <f>IF(675 - SUM(N29:DN29)&lt;0, 0, 675 - SUM(N29:DN29))</f>
+        <v>550</v>
       </c>
       <c r="AD31" s="60"/>
       <c r="AE31" s="60"/>
@@ -5154,7 +5155,7 @@
       <c r="L32" s="65"/>
       <c r="M32" s="65"/>
       <c r="N32" s="102" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O32" s="103"/>
       <c r="P32" s="103"/>
@@ -5171,8 +5172,8 @@
       <c r="AA32" s="103"/>
       <c r="AB32" s="104"/>
       <c r="AC32" s="101">
-        <f>IF(3-(COUNTIF(N28:DN28, "W"))&lt;0, 0, 3-(COUNTIF(N28:DN28, "W")))</f>
-        <v>3</v>
+        <f>IF(5-(COUNTIF(N28:DN28, "W"))&lt;0, 0, 5-(COUNTIF(N28:DN28, "W")))</f>
+        <v>4</v>
       </c>
       <c r="AD32" s="60"/>
       <c r="AE32" s="60"/>

</xml_diff>